<commit_message>
Added flavors and beer matches
</commit_message>
<xml_diff>
--- a/data/Archive/beermap.xlsx
+++ b/data/Archive/beermap.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="0" windowWidth="17000" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Big Style List" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5222" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5287" uniqueCount="1099">
   <si>
     <t>Color</t>
   </si>
@@ -3193,12 +3193,6 @@
     <t>BreweryDB id</t>
   </si>
   <si>
-    <t>94/95</t>
-  </si>
-  <si>
-    <t>81/102?</t>
-  </si>
-  <si>
     <t>14 or 15</t>
   </si>
   <si>
@@ -3206,6 +3200,129 @@
   </si>
   <si>
     <t>115/116</t>
+  </si>
+  <si>
+    <t>66/47</t>
+  </si>
+  <si>
+    <t>48/49/50/51</t>
+  </si>
+  <si>
+    <t>Bamberg-Style Helles (Smoke) Rauchbier Lager</t>
+  </si>
+  <si>
+    <t>1.044-1.050</t>
+  </si>
+  <si>
+    <t>1.008-1.012</t>
+  </si>
+  <si>
+    <t>3.8-4.4</t>
+  </si>
+  <si>
+    <t>45/56</t>
+  </si>
+  <si>
+    <t>60/64</t>
+  </si>
+  <si>
+    <t>32/28</t>
+  </si>
+  <si>
+    <t>37/29</t>
+  </si>
+  <si>
+    <t>22/33</t>
+  </si>
+  <si>
+    <t>94/95/112/113</t>
+  </si>
+  <si>
+    <t>1.060 – 1.090</t>
+  </si>
+  <si>
+    <t>30 – 60</t>
+  </si>
+  <si>
+    <t>10 – 22</t>
+  </si>
+  <si>
+    <t>1.015 – 1.022</t>
+  </si>
+  <si>
+    <t>6 – 9</t>
+  </si>
+  <si>
+    <t>1.080 – 1.120</t>
+  </si>
+  <si>
+    <t>35 – 70</t>
+  </si>
+  <si>
+    <t>8 – 22</t>
+  </si>
+  <si>
+    <t>8 – 12</t>
+  </si>
+  <si>
+    <t>1.018 – 1.030</t>
+  </si>
+  <si>
+    <t>1.016 – 1.030</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8 – 12</t>
+  </si>
+  <si>
+    <t>10 – 19</t>
+  </si>
+  <si>
+    <t>50 – 120</t>
+  </si>
+  <si>
+    <t>93/96</t>
+  </si>
+  <si>
+    <t>103/101</t>
+  </si>
+  <si>
+    <t>20-30</t>
+  </si>
+  <si>
+    <t>12-22</t>
+  </si>
+  <si>
+    <t>Classic Rauchbier</t>
+  </si>
+  <si>
+    <t>81/82/102?</t>
+  </si>
+  <si>
+    <t>54/85/86/87</t>
+  </si>
+  <si>
+    <t>40/46</t>
+  </si>
+  <si>
+    <t>25/27/74</t>
+  </si>
+  <si>
+    <t>1/3/6/10/73</t>
+  </si>
+  <si>
+    <t>78/92</t>
+  </si>
+  <si>
+    <t>117/118</t>
+  </si>
+  <si>
+    <t>75/77/106</t>
+  </si>
+  <si>
+    <t>19/38</t>
+  </si>
+  <si>
+    <t>89/100</t>
   </si>
 </sst>
 </file>
@@ -3428,7 +3545,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1393">
+  <cellStyleXfs count="1409">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4822,8 +4939,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4954,8 +5087,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1393">
+  <cellStyles count="1409">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5652,6 +5796,14 @@
     <cellStyle name="Followed Hyperlink" xfId="1388" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1390" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1408" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6348,6 +6500,14 @@
     <cellStyle name="Hyperlink" xfId="1387" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1389" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1407" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6677,10 +6837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6744,7 +6904,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>1055</v>
+        <v>1069</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1032</v>
@@ -6784,8 +6944,8 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4">
-        <v>93</v>
+      <c r="A4" t="s">
+        <v>1084</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>1033</v>
@@ -6866,8 +7026,8 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6">
-        <v>78</v>
+      <c r="A6" t="s">
+        <v>1094</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1035</v>
@@ -6957,8 +7117,8 @@
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9">
-        <v>75</v>
+      <c r="A9" t="s">
+        <v>1096</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>997</v>
@@ -7128,7 +7288,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>1056</v>
+        <v>1089</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>1001</v>
@@ -7177,8 +7337,8 @@
       <c r="I15" s="30"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16">
-        <v>103</v>
+      <c r="A16" t="s">
+        <v>1085</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>1002</v>
@@ -7312,8 +7472,8 @@
       <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20">
-        <v>89</v>
+      <c r="A20" t="s">
+        <v>1098</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1038</v>
@@ -7561,8 +7721,8 @@
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27">
-        <v>45</v>
+      <c r="A27" t="s">
+        <v>1064</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>71</v>
@@ -7603,7 +7763,7 @@
     </row>
     <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>1006</v>
@@ -7787,8 +7947,8 @@
       <c r="I33" s="30"/>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34">
-        <v>3</v>
+      <c r="A34" s="4" t="s">
+        <v>1093</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>1010</v>
@@ -8069,8 +8229,8 @@
       </c>
     </row>
     <row r="41" spans="1:21">
-      <c r="A41">
-        <v>22</v>
+      <c r="A41" t="s">
+        <v>1068</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>76</v>
@@ -8108,7 +8268,7 @@
     </row>
     <row r="42" spans="1:21" ht="16" thickBot="1">
       <c r="A42" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>1016</v>
@@ -8160,8 +8320,8 @@
       <c r="I43" s="30"/>
     </row>
     <row r="44" spans="1:21">
-      <c r="A44">
-        <v>25</v>
+      <c r="A44" t="s">
+        <v>1092</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>1017</v>
@@ -8198,8 +8358,8 @@
       </c>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45">
-        <v>32</v>
+      <c r="A45" t="s">
+        <v>1066</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>1018</v>
@@ -8236,8 +8396,8 @@
       </c>
     </row>
     <row r="46" spans="1:21">
-      <c r="A46">
-        <v>37</v>
+      <c r="A46" t="s">
+        <v>1067</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>14</v>
@@ -8289,6 +8449,9 @@
       <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:21">
+      <c r="A48">
+        <v>11</v>
+      </c>
       <c r="B48" s="9" t="s">
         <v>1019</v>
       </c>
@@ -8327,6 +8490,9 @@
       </c>
     </row>
     <row r="49" spans="1:13">
+      <c r="A49">
+        <v>12</v>
+      </c>
       <c r="B49" s="9" t="s">
         <v>1020</v>
       </c>
@@ -8365,6 +8531,9 @@
       </c>
     </row>
     <row r="50" spans="1:13">
+      <c r="A50">
+        <v>14</v>
+      </c>
       <c r="B50" s="10" t="s">
         <v>1021</v>
       </c>
@@ -8450,8 +8619,8 @@
       </c>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53">
-        <v>19</v>
+      <c r="A53" t="s">
+        <v>1097</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>7</v>
@@ -8747,7 +8916,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>1024</v>
@@ -8934,6 +9103,9 @@
       <c r="I66" s="30"/>
     </row>
     <row r="67" spans="1:13">
+      <c r="A67" t="s">
+        <v>1059</v>
+      </c>
       <c r="B67" s="9" t="s">
         <v>1039</v>
       </c>
@@ -9054,8 +9226,8 @@
       </c>
     </row>
     <row r="70" spans="1:13">
-      <c r="A70">
-        <v>118</v>
+      <c r="A70" t="s">
+        <v>1095</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>1040</v>
@@ -9280,8 +9452,8 @@
       <c r="I76" s="30"/>
     </row>
     <row r="77" spans="1:13">
-      <c r="A77">
-        <v>46</v>
+      <c r="A77" t="s">
+        <v>1091</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>1028</v>
@@ -9359,6 +9531,9 @@
       </c>
     </row>
     <row r="79" spans="1:13">
+      <c r="A79">
+        <v>57</v>
+      </c>
       <c r="B79" s="9" t="s">
         <v>1029</v>
       </c>
@@ -9397,8 +9572,8 @@
       </c>
     </row>
     <row r="80" spans="1:13">
-      <c r="A80">
-        <v>66</v>
+      <c r="A80" t="s">
+        <v>1058</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>1030</v>
@@ -9690,8 +9865,8 @@
       </c>
     </row>
     <row r="88" spans="1:14" ht="16" thickBot="1">
-      <c r="A88">
-        <v>64</v>
+      <c r="A88" t="s">
+        <v>1065</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>989</v>
@@ -9725,6 +9900,184 @@
       </c>
       <c r="L88" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14">
+      <c r="A89">
+        <v>54</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E89" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F89">
+        <v>18</v>
+      </c>
+      <c r="G89">
+        <v>25</v>
+      </c>
+      <c r="H89">
+        <v>4</v>
+      </c>
+      <c r="I89" s="16">
+        <v>5.5</v>
+      </c>
+      <c r="J89" t="s">
+        <v>331</v>
+      </c>
+      <c r="K89" t="s">
+        <v>343</v>
+      </c>
+      <c r="L89" t="s">
+        <v>119</v>
+      </c>
+      <c r="M89" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14">
+      <c r="A90" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C90" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="D90" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="E90" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="F90" s="57" t="s">
+        <v>1086</v>
+      </c>
+      <c r="H90" s="58" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J90" t="s">
+        <v>343</v>
+      </c>
+      <c r="K90" t="s">
+        <v>133</v>
+      </c>
+      <c r="L90" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14">
+      <c r="A91">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1073</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H91" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J91" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="K91" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="L91" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="M91" s="54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14">
+      <c r="A92">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>51</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H92" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J92" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="K92" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="L92" s="54" t="s">
+        <v>331</v>
+      </c>
+      <c r="M92" s="54" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="A93">
+        <v>34</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E93" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1083</v>
+      </c>
+      <c r="H93" t="s">
+        <v>1082</v>
+      </c>
+      <c r="J93" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="K93" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="L93" s="54" t="s">
+        <v>329</v>
+      </c>
+      <c r="M93" s="54" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -9742,8 +10095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ70"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
matched all the beers and flavors
</commit_message>
<xml_diff>
--- a/data/Archive/beermap.xlsx
+++ b/data/Archive/beermap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Big Style List" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5287" uniqueCount="1099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5286" uniqueCount="1098">
   <si>
     <t>Color</t>
   </si>
@@ -3193,9 +3193,6 @@
     <t>BreweryDB id</t>
   </si>
   <si>
-    <t>14 or 15</t>
-  </si>
-  <si>
     <t>43/16</t>
   </si>
   <si>
@@ -3298,9 +3295,6 @@
     <t>81/82/102?</t>
   </si>
   <si>
-    <t>54/85/86/87</t>
-  </si>
-  <si>
     <t>40/46</t>
   </si>
   <si>
@@ -3323,6 +3317,9 @@
   </si>
   <si>
     <t>89/100</t>
+  </si>
+  <si>
+    <t>85/86/87</t>
   </si>
 </sst>
 </file>
@@ -6839,8 +6836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6904,7 +6901,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>1032</v>
@@ -6945,7 +6942,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>1033</v>
@@ -7027,7 +7024,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>1035</v>
@@ -7118,7 +7115,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>997</v>
@@ -7288,7 +7285,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>1001</v>
@@ -7338,7 +7335,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>1002</v>
@@ -7473,7 +7470,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>1038</v>
@@ -7722,7 +7719,7 @@
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>71</v>
@@ -7763,7 +7760,7 @@
     </row>
     <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>1006</v>
@@ -7948,7 +7945,7 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="4" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>1010</v>
@@ -8230,7 +8227,7 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>76</v>
@@ -8267,8 +8264,8 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="16" thickBot="1">
-      <c r="A42" t="s">
-        <v>1055</v>
+      <c r="A42">
+        <v>15</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>1016</v>
@@ -8321,7 +8318,7 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>1017</v>
@@ -8359,7 +8356,7 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>1018</v>
@@ -8397,7 +8394,7 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>14</v>
@@ -8620,7 +8617,7 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>7</v>
@@ -8916,7 +8913,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>1024</v>
@@ -9104,7 +9101,7 @@
     </row>
     <row r="67" spans="1:13">
       <c r="A67" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>1039</v>
@@ -9227,7 +9224,7 @@
     </row>
     <row r="70" spans="1:13">
       <c r="A70" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B70" s="10" t="s">
         <v>1040</v>
@@ -9453,7 +9450,7 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>1028</v>
@@ -9573,7 +9570,7 @@
     </row>
     <row r="80" spans="1:13">
       <c r="A80" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>1030</v>
@@ -9866,7 +9863,7 @@
     </row>
     <row r="88" spans="1:14" ht="16" thickBot="1">
       <c r="A88" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>989</v>
@@ -9907,16 +9904,16 @@
         <v>54</v>
       </c>
       <c r="B89" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C89" t="s">
         <v>1060</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>1061</v>
       </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>1062</v>
-      </c>
-      <c r="E89" t="s">
-        <v>1063</v>
       </c>
       <c r="F89">
         <v>18</v>
@@ -9945,10 +9942,10 @@
     </row>
     <row r="90" spans="1:14">
       <c r="A90" t="s">
-        <v>1090</v>
+        <v>1097</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="C90" s="55" t="s">
         <v>194</v>
@@ -9960,10 +9957,10 @@
         <v>180</v>
       </c>
       <c r="F90" s="57" t="s">
+        <v>1085</v>
+      </c>
+      <c r="H90" s="58" t="s">
         <v>1086</v>
-      </c>
-      <c r="H90" s="58" t="s">
-        <v>1087</v>
       </c>
       <c r="J90" t="s">
         <v>343</v>
@@ -9983,19 +9980,19 @@
         <v>5</v>
       </c>
       <c r="C91" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F91" t="s">
         <v>1070</v>
       </c>
-      <c r="D91" t="s">
-        <v>1073</v>
-      </c>
-      <c r="E91" t="s">
-        <v>1074</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="H91" t="s">
         <v>1071</v>
-      </c>
-      <c r="H91" t="s">
-        <v>1072</v>
       </c>
       <c r="J91" s="54" t="s">
         <v>119</v>
@@ -10018,19 +10015,19 @@
         <v>51</v>
       </c>
       <c r="C92" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1077</v>
+      </c>
+      <c r="F92" t="s">
         <v>1075</v>
       </c>
-      <c r="D92" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E92" t="s">
-        <v>1078</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="H92" t="s">
         <v>1076</v>
-      </c>
-      <c r="H92" t="s">
-        <v>1077</v>
       </c>
       <c r="J92" s="54" t="s">
         <v>133</v>
@@ -10053,19 +10050,19 @@
         <v>11</v>
       </c>
       <c r="C93" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D93" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E93" t="s">
         <v>1080</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
+        <v>1082</v>
+      </c>
+      <c r="H93" t="s">
         <v>1081</v>
-      </c>
-      <c r="F93" t="s">
-        <v>1083</v>
-      </c>
-      <c r="H93" t="s">
-        <v>1082</v>
       </c>
       <c r="J93" s="54" t="s">
         <v>87</v>
@@ -10095,7 +10092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>

</xml_diff>